<commit_message>
BossTests hinzugefügt + GegnerTests Nummerierung Korrigiert + Requirements Boss hinzugefügt
</commit_message>
<xml_diff>
--- a/diagramme/GegnerTests.xlsx
+++ b/diagramme/GegnerTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/76fd2fc772ef66ad/Dokumente/UNI/Anfängerpraktikum/anfaengerpraktikum/diagramme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Desktop\UNI\S4\ComputerspielEntwicklung\DasSpiel\anfaengerpraktikum\diagramme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_AD4DB114E441178AC67DF45A5E13CB14693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DE72A8B-B3CD-4D31-9FC4-B4169A6B20DF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60A8BA9-4E5A-435B-8891-9DD954490793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Der Gegner muss eine leichte Attacke durchführen können</t>
   </si>
   <si>
-    <t>2.2.3.2.6</t>
-  </si>
-  <si>
     <t>2.2.3.3.1</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>2.2.3.5.2</t>
   </si>
 </sst>
 </file>
@@ -239,19 +239,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -529,22 +527,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
-    <col min="2" max="2" width="176.6328125" customWidth="1"/>
-    <col min="3" max="3" width="110.81640625" customWidth="1"/>
-    <col min="4" max="4" width="115.1796875" customWidth="1"/>
-    <col min="5" max="5" width="17.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="176.6640625" customWidth="1"/>
+    <col min="3" max="3" width="110.77734375" customWidth="1"/>
+    <col min="4" max="4" width="115.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -558,10 +556,10 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -569,16 +567,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -586,16 +584,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -603,148 +601,145 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="E5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E11" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>